<commit_message>
page artistes html->php +  images artistes
</commit_message>
<xml_diff>
--- a/donnees/baseDeDonnees.xlsx
+++ b/donnees/baseDeDonnees.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ETML\2020-2021\01-Projet\042-GesProj2\phptest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ETML\2020-2021\01-Projet\042-GesProj2\donnees\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70C5894-A60A-4EE2-9A4C-5FF9B97D03C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22110" yWindow="1680" windowWidth="21600" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="artistes" sheetId="1" r:id="rId1"/>
@@ -20,14 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -203,7 +196,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,7 +420,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Feuil1" xfId="1"/>
+    <cellStyle name="Normal_Feuil1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -738,16 +731,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -910,10 +904,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>